<commit_message>
Add make artificial data
</commit_message>
<xml_diff>
--- a/캡스톤 비용지출.xlsx
+++ b/캡스톤 비용지출.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\류형주\Desktop\git\CrimePrediction_PatrolAlgorithm\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19C1ECCC-B78B-448A-AD2F-FF21EDD95D3F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CD44963-5F32-4578-81AD-885E34C0643B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{4D0D9830-1457-41E7-A3DC-72562A2D1657}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="10">
   <si>
     <t>항목</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -549,7 +549,7 @@
   <dimension ref="B2:E20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -626,10 +626,16 @@
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.4">
-      <c r="B8" s="1"/>
+      <c r="B8" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="4"/>
+      <c r="D8" s="2">
+        <v>11200</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B9" s="1"/>
@@ -704,7 +710,7 @@
       <c r="C20" s="6"/>
       <c r="D20" s="7">
         <f>SUM(C4:C19) - SUM(D4:D19)</f>
-        <v>83500</v>
+        <v>72300</v>
       </c>
       <c r="E20" s="8"/>
     </row>

</xml_diff>

<commit_message>
Fix happy sushi day
</commit_message>
<xml_diff>
--- a/캡스톤 비용지출.xlsx
+++ b/캡스톤 비용지출.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\류형주\Desktop\git\CrimePrediction_PatrolAlgorithm\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\류형주\Desktop\git\crime-predict\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CD44963-5F32-4578-81AD-885E34C0643B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C5B092A-FF3F-4927-B99B-E1CB31611E99}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{4D0D9830-1457-41E7-A3DC-72562A2D1657}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="11">
   <si>
     <t>항목</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -73,6 +73,10 @@
   </si>
   <si>
     <t>V</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>무모한초밥</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -549,7 +553,7 @@
   <dimension ref="B2:E20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -638,10 +642,16 @@
       </c>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.4">
-      <c r="B9" s="1"/>
+      <c r="B9" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="4"/>
+      <c r="D9" s="2">
+        <v>31800</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B10" s="1"/>
@@ -710,7 +720,7 @@
       <c r="C20" s="6"/>
       <c r="D20" s="7">
         <f>SUM(C4:C19) - SUM(D4:D19)</f>
-        <v>72300</v>
+        <v>40500</v>
       </c>
       <c r="E20" s="8"/>
     </row>

</xml_diff>

<commit_message>
Fix arranged files and codes
</commit_message>
<xml_diff>
--- a/캡스톤 비용지출.xlsx
+++ b/캡스톤 비용지출.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\류형주\Desktop\git\crime-predict\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C5B092A-FF3F-4927-B99B-E1CB31611E99}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{692D54BB-551E-4672-8A57-CBADDA99193B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{4D0D9830-1457-41E7-A3DC-72562A2D1657}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="11">
   <si>
     <t>항목</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -553,7 +553,7 @@
   <dimension ref="B2:E20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="M15" sqref="M15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -654,10 +654,16 @@
       </c>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.4">
-      <c r="B10" s="1"/>
+      <c r="B10" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="4"/>
+      <c r="D10" s="2">
+        <v>13700</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B11" s="1"/>
@@ -720,7 +726,7 @@
       <c r="C20" s="6"/>
       <c r="D20" s="7">
         <f>SUM(C4:C19) - SUM(D4:D19)</f>
-        <v>40500</v>
+        <v>26800</v>
       </c>
       <c r="E20" s="8"/>
     </row>

</xml_diff>

<commit_message>
Upload ppt for manymany
</commit_message>
<xml_diff>
--- a/캡스톤 비용지출.xlsx
+++ b/캡스톤 비용지출.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\류형주\Desktop\git\crime-predict\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{692D54BB-551E-4672-8A57-CBADDA99193B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77A09ECE-D9CB-4037-99F2-A23A1259E1DD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{4D0D9830-1457-41E7-A3DC-72562A2D1657}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="14">
   <si>
     <t>항목</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -52,14 +52,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>류형주</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>김영서</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>만랩커피</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -77,6 +69,26 @@
   </si>
   <si>
     <t>무모한초밥</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>쭈꾸미불고기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>동연</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>영서</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>형주</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">  </t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -553,7 +565,7 @@
   <dimension ref="B2:E20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M15" sqref="M15"/>
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -582,12 +594,12 @@
         <v>3</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B4" s="1" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="C4" s="2">
         <v>50000</v>
@@ -597,19 +609,19 @@
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B5" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2">
         <v>6700</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B6" s="1" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="C6" s="2">
         <v>50000</v>
@@ -619,63 +631,73 @@
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B7" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2">
         <v>9800</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B8" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2">
         <v>11200</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B9" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2">
         <v>31800</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B10" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2">
         <v>13700</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.4">
-      <c r="B11" s="1"/>
-      <c r="C11" s="2"/>
+      <c r="B11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" s="2">
+        <v>50000</v>
+      </c>
       <c r="D11" s="2"/>
       <c r="E11" s="4"/>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.4">
-      <c r="B12" s="1"/>
+      <c r="B12" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="4"/>
+      <c r="D12" s="2">
+        <v>45000</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B13" s="1"/>
@@ -703,7 +725,9 @@
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B17" s="1"/>
-      <c r="C17" s="2"/>
+      <c r="C17" s="2" t="s">
+        <v>13</v>
+      </c>
       <c r="D17" s="2"/>
       <c r="E17" s="4"/>
     </row>
@@ -721,12 +745,12 @@
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B20" s="5" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C20" s="6"/>
       <c r="D20" s="7">
         <f>SUM(C4:C19) - SUM(D4:D19)</f>
-        <v>26800</v>
+        <v>31800</v>
       </c>
       <c r="E20" s="8"/>
     </row>

</xml_diff>